<commit_message>
mejoras tras navidad, redacción
</commit_message>
<xml_diff>
--- a/peer75.xlsx
+++ b/peer75.xlsx
@@ -473,12 +473,12 @@
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>26</v>
+        <v>17</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>26</v>
+        <v>17</v>
       </c>
     </row>
     <row r="28">
@@ -533,7 +533,7 @@
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>26</v>
+        <v>56</v>
       </c>
     </row>
     <row r="39">

</xml_diff>